<commit_message>
Added new columns and fixed one problem with Excel opening.
</commit_message>
<xml_diff>
--- a/Parameters/ProjectsSubTypes.xlsx
+++ b/Parameters/ProjectsSubTypes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\JNB\MLE\DES.LM.Reports\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DES.LM.Reports\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5505ABCA-43AF-4AE2-A875-2024E877CBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2E00C8-0448-4D69-8133-D307967FD4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
   <si>
     <t>А0172. Адм.время НУП. Отпуска</t>
   </si>
@@ -136,6 +136,30 @@
   </si>
   <si>
     <t>ProjectSubTypePart</t>
+  </si>
+  <si>
+    <t>А0210-НПУ. Адм. управление персоналом</t>
+  </si>
+  <si>
+    <t>А0264-Адм. время НСКК. Больничный</t>
+  </si>
+  <si>
+    <t>А0298 -Адм. Время. НРБ. Больничный</t>
+  </si>
+  <si>
+    <t>А0425 - Отгулы за ранее отработанное время (переработки)</t>
+  </si>
+  <si>
+    <t>А0426 - Отгулы за ранее отработанное время (переработки)</t>
+  </si>
+  <si>
+    <t>А0288-Адм. время. НИС. Управленческие</t>
+  </si>
+  <si>
+    <t>А0483 - Рабочее время в пути, связанное с командировками и т.п. (происходящие в рабочее время)</t>
+  </si>
+  <si>
+    <t>КомВПути</t>
   </si>
 </sst>
 </file>
@@ -191,10 +215,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -476,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F53492B-E9B6-44FD-A10D-37455B40CAC6}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,28 +606,28 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>12</v>
@@ -606,7 +635,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>12</v>
@@ -614,7 +643,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>12</v>
@@ -622,7 +651,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>12</v>
@@ -630,7 +659,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>12</v>
@@ -638,7 +667,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>12</v>
@@ -646,51 +675,51 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>22</v>
@@ -698,43 +727,163 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+      <c r="A30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>29</v>
       </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added all reports forms to the repository.
</commit_message>
<xml_diff>
--- a/Parameters/ProjectsSubTypes.xlsx
+++ b/Parameters/ProjectsSubTypes.xlsx
@@ -1,14 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DES.LM.Reports\Parameters\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2E00C8-0448-4D69-8133-D307967FD4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADDA915-8483-4157-814D-F1FBD2E46DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>